<commit_message>
Mapping de la partie corps entre modèle métier / CDA / FHIR (#89)
* Ajout des ressources CDA Corps

* Correction de l'erreur du type IVL_INT

* Delete input/fsh/MappingML_CDA_FHIR_Corps directory

* Stop tracking local working repositories

* Mapping entre ML/CDA/FHIR de la partie corps

* Création de nx mappings

* MAJ mapping suite review de NRISS

* MAJ mapping suite review de NRISS

* MAJ modèle logique corps

* MAJ de la requete sql pour récupération des mappings de l'entete

* Création de nouveaux mapping pour le corps

* Mapping de la partie corps entre ML/CDA/FHIR

* MAJ mapping corps

* Mise à jour du mapping et correction des erreurs liées dans le ML et ressources FHIR

* Correction erreurs suite review NRISS

* Mise à jour mapping de la partie corps b93eaabe33fade2419e69edaa53fc530a309162b
</commit_message>
<xml_diff>
--- a/main/ig/FRMediaLMCDAFHIR.xlsx
+++ b/main/ig/FRMediaLMCDAFHIR.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="77">
   <si>
     <t>Property</t>
   </si>
@@ -55,7 +55,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-23T08:28:04+00:00</t>
+    <t>2026-01-28T14:36:08+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>https://interop.esante.gouv.fr/ig/document/core/StructureDefinition/fr-media-document</t>
+  </si>
+  <si>
+    <t>FRMediaDocument</t>
   </si>
   <si>
     <t>FRMediaDocument.identifier</t>
@@ -738,7 +741,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -780,7 +783,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -793,7 +796,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
@@ -806,7 +809,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -819,7 +822,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -832,7 +835,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
@@ -845,7 +848,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -858,7 +861,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -871,7 +874,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
@@ -884,7 +887,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -897,7 +900,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -910,7 +913,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -923,7 +926,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -936,7 +939,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -946,6 +949,19 @@
         <v>75</v>
       </c>
       <c r="E15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="E16" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>